<commit_message>
Path Exist Logic Added
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/Config.xlsx
+++ b/BE_LTD_Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A33ACB16-0481-4EF2-A569-3B41FC996B5F}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DFC993A-A413-4C98-8E30-EF2DB05D3704}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\SummaryReport.xlsx</t>
+  </si>
+  <si>
+    <t>ToEmailAdress</t>
+  </si>
+  <si>
+    <t>sagarreddy.shyamala@bradsol.com</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -618,7 +624,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Created Folder With Current Date
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/Config.xlsx
+++ b/BE_LTD_Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DFC993A-A413-4C98-8E30-EF2DB05D3704}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E62957-225B-4EA2-8E17-37FA0CA4E18D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -167,6 +167,42 @@
   </si>
   <si>
     <t>sagarreddy.shyamala@bradsol.com</t>
+  </si>
+  <si>
+    <t>EmailSubject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statement </t>
+  </si>
+  <si>
+    <t>HDFC_Subject</t>
+  </si>
+  <si>
+    <t>ICICI_Subject</t>
+  </si>
+  <si>
+    <t>AXIS_Subject</t>
+  </si>
+  <si>
+    <t>SBI_Subject</t>
+  </si>
+  <si>
+    <t>Bank_Names</t>
+  </si>
+  <si>
+    <t>HDFC,AXIS,ICICI,SBI</t>
+  </si>
+  <si>
+    <t>HDFC Statement</t>
+  </si>
+  <si>
+    <t>ICICI Statement</t>
+  </si>
+  <si>
+    <t>AXIS Statement</t>
+  </si>
+  <si>
+    <t>SBI Statement</t>
   </si>
 </sst>
 </file>
@@ -544,7 +580,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -632,12 +668,54 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Extracted Pdf Payment Reference Number
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/Config.xlsx
+++ b/BE_LTD_Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E62957-225B-4EA2-8E17-37FA0CA4E18D}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{622AF42E-3795-4D52-8962-46A97EE57D0F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -169,40 +169,10 @@
     <t>sagarreddy.shyamala@bradsol.com</t>
   </si>
   <si>
-    <t>EmailSubject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statement </t>
-  </si>
-  <si>
-    <t>HDFC_Subject</t>
-  </si>
-  <si>
-    <t>ICICI_Subject</t>
-  </si>
-  <si>
-    <t>AXIS_Subject</t>
-  </si>
-  <si>
-    <t>SBI_Subject</t>
-  </si>
-  <si>
-    <t>Bank_Names</t>
-  </si>
-  <si>
-    <t>HDFC,AXIS,ICICI,SBI</t>
-  </si>
-  <si>
-    <t>HDFC Statement</t>
-  </si>
-  <si>
-    <t>ICICI Statement</t>
-  </si>
-  <si>
-    <t>AXIS Statement</t>
-  </si>
-  <si>
-    <t>SBI Statement</t>
+    <t>BankNames</t>
+  </si>
+  <si>
+    <t>Hdfc,Axis</t>
   </si>
 </sst>
 </file>
@@ -577,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -676,46 +646,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1693,12 +1628,6 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Extracted Total Amount From Pdf
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/Config.xlsx
+++ b/BE_LTD_Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{622AF42E-3795-4D52-8962-46A97EE57D0F}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{191BE4CD-E85F-4128-B99D-7F62D70D5504}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>BankNames</t>
+  </si>
+  <si>
+    <t>EmailFolder</t>
+  </si>
+  <si>
+    <t>Biological E Ltd</t>
   </si>
   <si>
     <t>Hdfc,Axis</t>
@@ -550,7 +556,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -643,10 +649,17 @@
         <v>48</v>
       </c>
       <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
         <v>49</v>
       </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added Send Email To User
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/Config.xlsx
+++ b/BE_LTD_Dispatcher/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C8B8014-6561-4394-84E3-6AA533BE9D1B}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4AC65B2-7A43-4DF3-9EC6-A36A5E3FFED4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -154,55 +154,109 @@
     <t>SummaryReportFilePath</t>
   </si>
   <si>
-    <t>UnprotectedAttachmentsPath</t>
-  </si>
-  <si>
     <t>ToEmailAdress</t>
   </si>
   <si>
+    <t>EmailFolder</t>
+  </si>
+  <si>
+    <t>Biological E Ltd</t>
+  </si>
+  <si>
+    <t>SummaryReport</t>
+  </si>
+  <si>
+    <t>SummaryReportName</t>
+  </si>
+  <si>
+    <t>Axis Bank</t>
+  </si>
+  <si>
+    <t>PaymentReferenceNumber</t>
+  </si>
+  <si>
+    <t>(?&lt;=:\s)[0-9]{10}</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>(INR) \d+(,\d+)*(\.\d+)</t>
+  </si>
+  <si>
+    <t>CurrentDate</t>
+  </si>
+  <si>
+    <t>MM-dd-yyyy</t>
+  </si>
+  <si>
     <t>sagarreddy.shyamala@bradsol.com</t>
   </si>
   <si>
-    <t>BankNames</t>
-  </si>
-  <si>
-    <t>EmailFolder</t>
-  </si>
-  <si>
-    <t>Biological E Ltd</t>
+    <t>ClosingApplications</t>
+  </si>
+  <si>
+    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\Input\</t>
+  </si>
+  <si>
+    <t>Send_StartEmailNotificationBody</t>
+  </si>
+  <si>
+    <t>Send_StartEmailNotificationSubject</t>
+  </si>
+  <si>
+    <t>BE_LTD AXIS Process Started</t>
+  </si>
+  <si>
+    <t>Send_CompletedEmailNotificationBody</t>
+  </si>
+  <si>
+    <t>Send_CompletedEmailNotificationSubject</t>
+  </si>
+  <si>
+    <t>BE_LTD AXIS Process Completed</t>
+  </si>
+  <si>
+    <t>UnreadEmailsNotfoundBody</t>
+  </si>
+  <si>
+    <t>UnreadEmailsNotfoundSubject</t>
+  </si>
+  <si>
+    <t>BE_LTD AXIS Process-UnreadEmailsNotfound</t>
+  </si>
+  <si>
+    <t>AttachmentsNotFoundSubject</t>
+  </si>
+  <si>
+    <t>AttachmentsNotFoundBody</t>
+  </si>
+  <si>
+    <t>BE_LTD AXIS Process -AttachmentsNotFound</t>
+  </si>
+  <si>
+    <t>Hello Team, &lt;p&gt;This is to notify you that our BOT started the process for "Axis UTR Automation" .&lt;p&gt;Thanks &amp; Regards,&lt;p&gt;BE Ltd.</t>
+  </si>
+  <si>
+    <t>Hello Team,&lt;p&gt;This is to notify you that our BOT successfully completed the process for "Axis UTR Automation".&lt;p&gt;Thanks &amp; Regards,&lt;p&gt;BE Ltd.</t>
+  </si>
+  <si>
+    <t>Hello Team,&lt;p&gt;This is to notify you that our BOT couldn’t find any attachments for the process of "Axis UTR Automation".&lt;p&gt;Thanks &amp; Regards,&lt;p&gt;BE Ltd.</t>
+  </si>
+  <si>
+    <t>Hello Team,&lt;p&gt;This is to notify you that our BOT couldn’t find any unread emails for the process of "Axis UTR Automation".&lt;p&gt;Thanks &amp; Regards,&lt;p&gt;BE Ltd.</t>
+  </si>
+  <si>
+    <t>Excel,msedge,Acrobat.exe</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>FinalSummaryReportFilePath</t>
   </si>
   <si>
     <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\</t>
-  </si>
-  <si>
-    <t>SummaryReport</t>
-  </si>
-  <si>
-    <t>SummaryReportName</t>
-  </si>
-  <si>
-    <t>Excel</t>
-  </si>
-  <si>
-    <t>CloseExcelApplication</t>
-  </si>
-  <si>
-    <t>CloseEdgeApplication</t>
-  </si>
-  <si>
-    <t>CloseAdobeAcrobatApplication</t>
-  </si>
-  <si>
-    <t>msedge</t>
-  </si>
-  <si>
-    <t>Acrobat.exe</t>
-  </si>
-  <si>
-    <t>Axis Bank</t>
-  </si>
-  <si>
-    <t>,HDFC,AXIS,ICICI</t>
   </si>
 </sst>
 </file>
@@ -254,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -263,6 +317,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,16 +633,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="107.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="137.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -641,7 +697,7 @@
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -649,12 +705,12 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -662,83 +718,146 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1694,8 +1813,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Send Mail Reusable Task
</commit_message>
<xml_diff>
--- a/BE_LTD_Dispatcher/Data/Config.xlsx
+++ b/BE_LTD_Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bradsol-my.sharepoint.com/personal/sagarreddy_shyamala_bradsol_com/Documents/Documents/GitHub/brad-uipath/BE_LTD_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4AC65B2-7A43-4DF3-9EC6-A36A5E3FFED4}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0D325E7-1617-49F3-8E23-2334840AEB32}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -257,13 +257,49 @@
   </si>
   <si>
     <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BE_LTD_Dispatcher\Data\</t>
+  </si>
+  <si>
+    <t>Reusable_Tasks_Path</t>
+  </si>
+  <si>
+    <t>C:\Users\TEMP\OneDrive - bradsol.com\Documents\GitHub\brad-uipath\BRADSOL_Reusable_Tasks\</t>
+  </si>
+  <si>
+    <t>https://outlook.office.com/mail/</t>
+  </si>
+  <si>
+    <t>ExchangeDomain</t>
+  </si>
+  <si>
+    <t>SMTPServer</t>
+  </si>
+  <si>
+    <t>smtp.gmail.com</t>
+  </si>
+  <si>
+    <t>SMTPPortNumber</t>
+  </si>
+  <si>
+    <t>ToEmail</t>
+  </si>
+  <si>
+    <t>vidyasagarrpa@gmail.com</t>
+  </si>
+  <si>
+    <t>FromMail</t>
+  </si>
+  <si>
+    <t>OUTLOOK</t>
+  </si>
+  <si>
+    <t>Mail_Environment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -287,6 +323,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -308,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -319,6 +362,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z979"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -781,73 +825,42 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>58</v>
+      <c r="A14" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>60</v>
+      <c r="A15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>71</v>
+      <c r="A16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>63</v>
+      <c r="A17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1805,14 +1818,6 @@
     <row r="977" ht="14.25" customHeight="1"/>
     <row r="978" ht="14.25" customHeight="1"/>
     <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1824,14 +1829,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="2" max="2" width="130.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -2006,17 +2011,94 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28">
+        <v>587</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>